<commit_message>
Change csv const variable name Add 03 - プログラム file
</commit_message>
<xml_diff>
--- a/Steps/01 - 仮日程.xlsx
+++ b/Steps/01 - 仮日程.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user1/Barrabas/AA-Git/240521-test-form/240521-test-form/Steps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0230ABC9-A9C4-7044-AD42-9B132822C7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEDB744-9B13-9A4F-8D82-60AEA3A57C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="2180" windowWidth="26840" windowHeight="15580" activeTab="3" xr2:uid="{DA49BD13-D127-8D43-BF02-0A84109475CD}"/>
+    <workbookView xWindow="1580" yWindow="2180" windowWidth="26840" windowHeight="15580" activeTab="2" xr2:uid="{DA49BD13-D127-8D43-BF02-0A84109475CD}"/>
   </bookViews>
   <sheets>
     <sheet name="PriceRef" sheetId="3" r:id="rId1"/>
     <sheet name="EventRef" sheetId="1" r:id="rId2"/>
     <sheet name="仮日程" sheetId="4" r:id="rId3"/>
-    <sheet name="X - 大会要項Columns - X " sheetId="8" r:id="rId4"/>
+    <sheet name="X - 大会要項Columns - X " sheetId="8" state="hidden" r:id="rId4"/>
     <sheet name="大会要項の仮日程" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
@@ -2938,8 +2938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C84471-8F62-1042-A308-366AA5657EC1}">
   <dimension ref="A1:I501"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19700,7 +19700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44BEDFEC-A164-2645-B5F8-B549AB8B97BE}">
   <dimension ref="B3:F506"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
@@ -30763,7 +30763,7 @@
   <dimension ref="B1:F74"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>